<commit_message>
Modified tests v.3.5.0 and updated bag report
</commit_message>
<xml_diff>
--- a/Bag report.xlsx
+++ b/Bag report.xlsx
@@ -60,7 +60,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">1)Запустить тест </t>
+      <t xml:space="preserve">1) Запустить тест </t>
     </r>
     <r>
       <rPr>
@@ -120,7 +120,7 @@
         <rFont val="XO Thames"/>
         <sz val="12"/>
       </rPr>
-      <t xml:space="preserve">1)Запустить тест </t>
+      <t xml:space="preserve">1) Запустить тест </t>
     </r>
     <r>
       <rPr>
@@ -167,6 +167,145 @@
         <sz val="12"/>
       </rPr>
       <t>2) Раздел Editing Claims. Заполнение поля Description не валидными значениями.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t xml:space="preserve">Раздел News. Переход в раздел </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>Control Panel. Проверка раздела Creating News</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t xml:space="preserve">ОС Windows 10. </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>Android Studio Dolphin | 2021.3.1 Patch. AP I 29. Приложение на английском языке</t>
+    </r>
+  </si>
+  <si>
+    <t>1) Перейти в раздел News.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <color rgb="0000FF" tint="0"/>
+        <sz val="12"/>
+        <u val="single"/>
+      </rPr>
+      <t>https://photos.app.goo.gl/QQFFuKMFYTnt4SsDA</t>
+    </r>
+  </si>
+  <si>
+    <t>2) Перейти в раздел Control Panel.</t>
+  </si>
+  <si>
+    <t>3) Перейти в раздел Creatin News</t>
+  </si>
+  <si>
+    <t>4) Нажать на поле Category</t>
+  </si>
+  <si>
+    <t>Открылось всплывающее меню с выбором категорий на английском языке.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>Открылось всплывающее меню с выбором категорий на русском языке.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t xml:space="preserve">Раздел News. Переход в раздел </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>Control Panel. Проверка раздела Filter News.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>1) Перейти в раздел News.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <color rgb="0000FF" tint="0"/>
+        <sz val="12"/>
+        <u val="single"/>
+      </rPr>
+      <t>https://photos.app.goo.gl/P1fFoRHGpX2a8v2LA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>2) Перейти в раздел Control Panel.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>3) Перейти в раздел Filter News</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>4) Нажать на поле Category</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="XO Thames"/>
+        <sz val="12"/>
+      </rPr>
+      <t>Открылось всплывающее меню с выбором категорий на английском языке.</t>
     </r>
   </si>
 </sst>
@@ -210,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf applyFont="true" borderId="0" fillId="0" fontId="1" quotePrefix="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf applyFont="true" borderId="0" fillId="0" fontId="1" quotePrefix="false"/>
     <xf applyAlignment="true" applyFont="true" borderId="0" fillId="0" fontId="1" quotePrefix="false">
       <alignment horizontal="center" wrapText="true"/>
@@ -224,7 +363,6 @@
     <xf applyAlignment="true" applyFont="true" borderId="0" fillId="0" fontId="2" quotePrefix="false">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" quotePrefix="false"/>
     <xf applyAlignment="true" applyFont="true" borderId="0" fillId="0" fontId="1" quotePrefix="false">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -348,16 +486,19 @@
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
+          <a:prstDash val="solid"/>
         </a:ln>
         <a:ln>
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
+          <a:prstDash val="solid"/>
         </a:ln>
         <a:ln>
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
+          <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -497,13 +638,14 @@
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C2" s="0" t="n"/>
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -519,7 +661,7 @@
     <row outlineLevel="0" r="3">
       <c r="A3" s="2" t="s"/>
       <c r="B3" s="1" t="s"/>
-      <c r="C3" s="5" t="s"/>
+      <c r="C3" s="0" t="s"/>
       <c r="D3" s="2" t="s"/>
       <c r="E3" s="3" t="s"/>
       <c r="F3" s="2" t="s">
@@ -536,7 +678,8 @@
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="0" t="n"/>
+      <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -558,8 +701,8 @@
     <row outlineLevel="0" r="5">
       <c r="A5" s="2" t="s"/>
       <c r="B5" s="2" t="s"/>
-      <c r="C5" s="5" t="s"/>
-      <c r="D5" s="6" t="s"/>
+      <c r="C5" s="0" t="s"/>
+      <c r="D5" s="5" t="s"/>
       <c r="E5" s="2" t="s"/>
       <c r="F5" s="2" t="s">
         <v>23</v>
@@ -568,28 +711,152 @@
       <c r="H5" s="2" t="s"/>
       <c r="I5" s="4" t="s"/>
     </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="2" t="s"/>
+      <c r="B7" s="2" t="s"/>
+      <c r="D7" s="2" t="s"/>
+      <c r="E7" s="2" t="s"/>
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="4" t="s"/>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="2" t="s"/>
+      <c r="B8" s="2" t="s"/>
+      <c r="D8" s="2" t="s"/>
+      <c r="E8" s="2" t="s"/>
+      <c r="F8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="4" t="s"/>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="A9" s="2" t="s"/>
+      <c r="B9" s="2" t="s"/>
+      <c r="D9" s="2" t="s"/>
+      <c r="E9" s="2" t="s"/>
+      <c r="F9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="4" t="s"/>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="A10" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="A11" s="2" t="s"/>
+      <c r="B11" s="2" t="s"/>
+      <c r="D11" s="2" t="s"/>
+      <c r="E11" s="2" t="s"/>
+      <c r="F11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="4" t="s"/>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="A12" s="2" t="s"/>
+      <c r="B12" s="2" t="s"/>
+      <c r="D12" s="2" t="s"/>
+      <c r="E12" s="2" t="s"/>
+      <c r="F12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="4" t="s"/>
+    </row>
+    <row outlineLevel="0" r="13">
+      <c r="A13" s="2" t="s"/>
+      <c r="B13" s="2" t="s"/>
+      <c r="D13" s="2" t="s"/>
+      <c r="E13" s="2" t="s"/>
+      <c r="F13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="4" t="s"/>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="26">
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="C2:C3"/>
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="C4:C5"/>
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="D6:D9"/>
+    <mergeCell ref="E6:E9"/>
+    <mergeCell ref="I6:I9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="E10:E13"/>
+    <mergeCell ref="I10:I13"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink display="https://photos.app.goo.gl/y1MGzna7akeckcNa8" r:id="rId1" ref="I2"/>
-    <hyperlink display="https://photos.app.goo.gl/fqBRrSpaWKwSFsF7A" r:id="rId2" ref="I4"/>
+    <hyperlink display="https://photos.app.goo.gl/P1fFoRHGpX2a8v2LA" r:id="rId1" ref="I10"/>
+    <hyperlink display="https://photos.app.goo.gl/y1MGzna7akeckcNa8" r:id="rId2" ref="I2"/>
+    <hyperlink display="https://photos.app.goo.gl/fqBRrSpaWKwSFsF7A" r:id="rId3" ref="I4"/>
+    <hyperlink display="https://photos.app.goo.gl/QQFFuKMFYTnt4SsDA" r:id="rId4" ref="I6"/>
   </hyperlinks>
   <pageMargins bottom="0.790000021457672" footer="0.19680555164814" header="0.19680555164814" left="0.790000021457672" right="0.790000021457672" top="0.790000021457672"/>
 </worksheet>

</xml_diff>